<commit_message>
Tweak to exposure xlsx file.
</commit_message>
<xml_diff>
--- a/Inputs/PFOA_template_parameters_Exposure.xlsx
+++ b/Inputs/PFOA_template_parameters_Exposure.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/schlosser_paul_epa_gov/Documents/mcsim-5.6.5/template_montecarlo/pbpk_template_project/Inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa.sharepoint.com/sites/ORD/pkwg/Shared Documents/PFAS/PFAS inhalation/pfas_inhalation_pbpk/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="480" documentId="14_{BC2287C1-70F4-4BAE-BA85-F3EC3C708A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44F14544-4507-41B0-8362-3E258942B9C7}"/>
+  <xr:revisionPtr revIDLastSave="482" documentId="14_{BC2287C1-70F4-4BAE-BA85-F3EC3C708A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1987DEA-A4B2-4724-A204-1272800325CF}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="300" windowWidth="23415" windowHeight="13305" tabRatio="668" firstSheet="3" activeTab="3" xr2:uid="{089E7848-11EB-427A-89EA-83825F220BA0}"/>
+    <workbookView xWindow="-27195" yWindow="19590" windowWidth="25560" windowHeight="12930" tabRatio="668" activeTab="2" xr2:uid="{089E7848-11EB-427A-89EA-83825F220BA0}"/>
   </bookViews>
   <sheets>
     <sheet name="MKemperOral25BW" sheetId="11" r:id="rId1"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="138">
   <si>
     <t>Code</t>
   </si>
@@ -575,12 +575,18 @@
   <si>
     <t>Corresponds to a 61.5 day-old male Sprague-Dawley rat (i.e., almost 9 weeks old) based on the NTP growth curve (NTP_BW_SD.csv). Value was used in MPPD to estimate particle deposition.</t>
   </si>
+  <si>
+    <t>&lt;== actual dose from Table 9 of Kemper, 1 mg/kg target</t>
+  </si>
+  <si>
+    <t>&lt;== actual dose from Table 9 of Kemper, 5 mg/kg target</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -632,12 +638,6 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1612,7 +1612,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1943,7 +1943,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="G21" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2148,8 +2148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14E7732-3851-459F-8542-D34FCE787B60}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2480,7 +2480,7 @@
         <v>4.72</v>
       </c>
       <c r="G21" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2685,7 +2685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3765E89-16BD-455C-A068-3F9042142D87}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21:M23"/>
     </sheetView>
   </sheetViews>
@@ -6779,6 +6779,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C107526348C97345843FB1F7E3F5FF14" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1022ded5d06c8e179fc5cb1f37040178">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="2ba80736-48fa-4d73-aaff-bacaeeed013a" xmlns:ns6="41d9f072-86bf-4c63-b117-debf50ff4701" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="edea5721ce64dde47a72ba01132ba27b" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7251,20 +7265,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7311,7 +7311,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5B6850C-32F9-4402-840F-018327152438}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DC26B68-A11F-428F-9051-23DC6334A810}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7323,9 +7327,24 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DC26B68-A11F-428F-9051-23DC6334A810}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5B6850C-32F9-4402-840F-018327152438}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="2ba80736-48fa-4d73-aaff-bacaeeed013a"/>
+    <ds:schemaRef ds:uri="41d9f072-86bf-4c63-b117-debf50ff4701"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7340,6 +7359,7 @@
     <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
     <ds:schemaRef ds:uri="93237db7-bebb-43bb-9414-bc3313990c09"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="2ba80736-48fa-4d73-aaff-bacaeeed013a"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>